<commit_message>
==CALCULADORA CIENTIFICA=== ==CAMBIÓ A SER SOBRE LAS CONVERSIONES=== -Adiciones:     -Funciones para cada ventana de conversión     -Funcion de cubo (y su respectiva funcion de calculo), para la funcion de volumen     -Funcion de Prisma (y su respectiva funcion de calculo), para la funcion de volumen     -Funcion de Cilindro (y su respectiva funcion de calculo), para la funcion de volumen     -Funcion de Esfera (y su respectiva funcion de calculo), para la funcion de volumen     -Funcion de Cono (y su respectiva funcion de calculo), para la funcion de volumen     -Funcion de Piramide (y su respectiva funcion de calculo), para la funcion de volumen     -Ventana Volumem Completa     -Eliminacion de la mayoría de extras, quedando solo 3(volumen, temperatura, tiempo)
-Cambios:
    -ELIMINACIÓN DEL MENU DE CALCULADORAS Y LA CALCULADORA CIENTIFICA(decidí ser feliz)
    -NOS QUEDAMOS SOLO CON VOLUMEN
</commit_message>
<xml_diff>
--- a/archives/Idiomas.xlsx
+++ b/archives/Idiomas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Practicas\PythonPrjcts\the-calculator\archives\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556EE497-4881-48AF-A668-CB3CD8997B87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE16566-D92B-46FB-8BF6-28F92E56B237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="92">
   <si>
     <t>ID</t>
   </si>
@@ -90,9 +90,6 @@
     <t>GO_TO_MAIN_MENU</t>
   </si>
   <si>
-    <t>&amp;Conversiones</t>
-  </si>
-  <si>
     <t>Volumen</t>
   </si>
   <si>
@@ -144,9 +141,6 @@
     <t>Main menu</t>
   </si>
   <si>
-    <t>Conversions</t>
-  </si>
-  <si>
     <t>Volume</t>
   </si>
   <si>
@@ -223,6 +217,90 @@
   </si>
   <si>
     <t>Scientific</t>
+  </si>
+  <si>
+    <t>&amp;Extra</t>
+  </si>
+  <si>
+    <t>ARISTAS</t>
+  </si>
+  <si>
+    <t>Aristas</t>
+  </si>
+  <si>
+    <t>Edges</t>
+  </si>
+  <si>
+    <t>CUBO</t>
+  </si>
+  <si>
+    <t>Cubo</t>
+  </si>
+  <si>
+    <t>Cube</t>
+  </si>
+  <si>
+    <t>ACEPTAR</t>
+  </si>
+  <si>
+    <t>Aceptar</t>
+  </si>
+  <si>
+    <t>Ok</t>
+  </si>
+  <si>
+    <t>PRISMA</t>
+  </si>
+  <si>
+    <t>ESFERA</t>
+  </si>
+  <si>
+    <t>CONO</t>
+  </si>
+  <si>
+    <t>PIRAMIDE</t>
+  </si>
+  <si>
+    <t>FIGURA</t>
+  </si>
+  <si>
+    <t>Prisma Rectangular</t>
+  </si>
+  <si>
+    <t>Esfera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cono </t>
+  </si>
+  <si>
+    <t>Figura</t>
+  </si>
+  <si>
+    <t>Rectangular Prism</t>
+  </si>
+  <si>
+    <t>Sphere</t>
+  </si>
+  <si>
+    <t>Cone</t>
+  </si>
+  <si>
+    <t>Pyramid</t>
+  </si>
+  <si>
+    <t>Pirámide</t>
+  </si>
+  <si>
+    <t>Figure</t>
+  </si>
+  <si>
+    <t>CILINDRO</t>
+  </si>
+  <si>
+    <t>Cilindro</t>
+  </si>
+  <si>
+    <t>Cylinder</t>
   </si>
 </sst>
 </file>
@@ -263,7 +341,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -327,6 +405,48 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -343,7 +463,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -354,11 +474,19 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -639,17 +767,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -664,14 +792,14 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>37</v>
+      <c r="B2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -679,10 +807,10 @@
         <v>20</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -690,10 +818,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -701,21 +829,21 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>39</v>
+      <c r="C6" s="11" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -723,10 +851,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -734,10 +862,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D8" s="2"/>
     </row>
@@ -746,10 +874,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -757,10 +885,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -768,10 +896,10 @@
         <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -779,10 +907,10 @@
         <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E12" s="2"/>
     </row>
@@ -791,10 +919,10 @@
         <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -802,10 +930,10 @@
         <v>14</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -813,10 +941,10 @@
         <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -824,21 +952,21 @@
         <v>16</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>50</v>
+      <c r="C17" s="11" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -846,10 +974,10 @@
         <v>18</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -857,130 +985,220 @@
         <v>19</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="13" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="11" t="s">
+      <c r="B21" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="12" t="s">
+      <c r="B22" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="11" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="12" t="s">
+      <c r="B23" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="11" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="12" t="s">
+      <c r="B24" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="11" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="12" t="s">
+      <c r="B25" s="9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="11" t="s">
+      <c r="C25" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="12" t="s">
+      <c r="B26" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="11" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B27" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="11" t="s">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="12" t="s">
+      <c r="B28" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="11" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="11" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="B27" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="12" t="s">
+      <c r="B29" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="8"/>
+      <c r="A30" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="8"/>
+      <c r="A31" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="8"/>
+      <c r="A32" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>91</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>